<commit_message>
fix pattern & with in TestAllQueries1
</commit_message>
<xml_diff>
--- a/Tests/TestingErrors.xlsx
+++ b/Tests/TestingErrors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
   <si>
     <t>Source File</t>
   </si>
@@ -122,10 +122,10 @@
     <t>Issue-Explain</t>
   </si>
   <si>
-    <t>StmtLst is not a valid result type</t>
-  </si>
-  <si>
-    <t>Same as above</t>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Stmt 4 is not assign type</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1087,9 +1087,6 @@
         <v>68</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
@@ -1103,9 +1100,7 @@
         <v>77</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="F22" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
@@ -1217,7 +1212,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
@@ -1230,8 +1225,11 @@
       <c r="D34" s="5">
         <v>123</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>30</v>
       </c>
@@ -1244,152 +1242,227 @@
       <c r="D36" s="5">
         <v>136</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="D37" s="3">
         <v>139</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="D38" s="3">
         <v>140</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="D39" s="3">
         <v>141</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="D40" s="3">
         <v>146</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="D41" s="3">
         <v>147</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="D42" s="3">
         <v>148</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="D43" s="3">
         <v>149</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="D44" s="3">
         <v>153</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="D45" s="3">
         <v>154</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="D46" s="3">
         <v>155</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="D47" s="3">
         <v>160</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="D48" s="3">
         <v>161</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="D49" s="3">
         <v>162</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="D50" s="3">
         <v>166</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="D51" s="3">
         <v>167</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="D52" s="3">
         <v>169</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="D53" s="3">
         <v>171</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="D54" s="3">
         <v>175</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="D55" s="3">
         <v>179</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="D56" s="3">
         <v>181</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="D57" s="3">
         <v>183</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="D58" s="3">
         <v>184</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="D59" s="3">
         <v>185</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="D60" s="3">
         <v>186</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update TestingErrors excel file
</commit_message>
<xml_diff>
--- a/Tests/TestingErrors.xlsx
+++ b/Tests/TestingErrors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="33">
   <si>
     <t>Source File</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>Stmt 4 is not assign type</t>
   </si>
 </sst>
 </file>
@@ -805,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1209,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
@@ -1229,7 +1226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>30</v>
       </c>
@@ -1242,11 +1239,11 @@
       <c r="D36" s="5">
         <v>136</v>
       </c>
-      <c r="F36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="D37" s="3">
         <v>139</v>
@@ -1255,7 +1252,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="D38" s="3">
         <v>140</v>
@@ -1264,7 +1261,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="D39" s="3">
         <v>141</v>
@@ -1273,7 +1270,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="D40" s="3">
         <v>146</v>
@@ -1282,7 +1279,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="D41" s="3">
         <v>147</v>
@@ -1291,7 +1288,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="D42" s="3">
         <v>148</v>
@@ -1300,7 +1297,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="D43" s="3">
         <v>149</v>
@@ -1309,7 +1306,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="D44" s="3">
         <v>153</v>
@@ -1318,7 +1315,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="D45" s="3">
         <v>154</v>
@@ -1327,7 +1324,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="D46" s="3">
         <v>155</v>
@@ -1336,7 +1333,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="D47" s="3">
         <v>160</v>
@@ -1345,7 +1342,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="D48" s="3">
         <v>161</v>

</xml_diff>

<commit_message>
uses solved outputs answer.
</commit_message>
<xml_diff>
--- a/Tests/TestingErrors.xlsx
+++ b/Tests/TestingErrors.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\NUS YEAR 4 SEM1\CS3202\cs3202-team-4-repo\Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="15600" tabRatio="500"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="25">
   <si>
     <t>Source File</t>
   </si>
@@ -336,6 +341,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,12 +361,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="105">
@@ -802,21 +807,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.625" customWidth="1"/>
     <col min="4" max="4" width="29.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="24.625" style="3" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -836,8 +841,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -852,12 +857,12 @@
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="14"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -870,10 +875,10 @@
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="14"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
@@ -886,10 +891,10 @@
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="14"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -902,10 +907,10 @@
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="14"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
@@ -918,10 +923,10 @@
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="14"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -934,10 +939,10 @@
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
-      <c r="A8" s="14"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
@@ -947,12 +952,12 @@
       <c r="D8" s="5">
         <v>19</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -962,10 +967,10 @@
       <c r="D9" s="5">
         <v>20</v>
       </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="14"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -975,10 +980,10 @@
       <c r="D10" s="5">
         <v>22</v>
       </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="14"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -988,10 +993,10 @@
       <c r="D11" s="5">
         <v>23</v>
       </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="14"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
@@ -1001,10 +1006,10 @@
       <c r="D12" s="5">
         <v>24</v>
       </c>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="14"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
       <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
@@ -1014,9 +1019,9 @@
       <c r="D13" s="5">
         <v>25</v>
       </c>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F13" s="15"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1030,8 +1035,8 @@
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1043,12 +1048,12 @@
       <c r="D17" s="5">
         <v>60</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="15"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1058,14 +1063,14 @@
       <c r="D18" s="5">
         <v>77</v>
       </c>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="15"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1077,12 +1082,12 @@
       <c r="D21" s="5">
         <v>68</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="11"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
@@ -1092,10 +1097,13 @@
       <c r="D22" s="5">
         <v>77</v>
       </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="12" t="s">
+      <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1108,8 +1116,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="12"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25" s="4" t="s">
         <v>3</v>
       </c>
@@ -1120,8 +1128,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="12"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
       <c r="B26" s="4" t="s">
         <v>3</v>
       </c>
@@ -1132,8 +1140,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="12"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
@@ -1144,8 +1152,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="12"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
       <c r="B28" s="4" t="s">
         <v>3</v>
       </c>
@@ -1156,8 +1164,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="12"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
       <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
@@ -1168,8 +1176,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="12"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
       <c r="B30" s="4" t="s">
         <v>3</v>
       </c>
@@ -1180,8 +1188,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="12"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31" s="4" t="s">
         <v>3</v>
       </c>
@@ -1192,8 +1200,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="12"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32" s="4" t="s">
         <v>3</v>
       </c>
@@ -1204,8 +1212,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="16" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -1224,8 +1232,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="16"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
       <c r="B35" s="4" t="s">
         <v>23</v>
       </c>
@@ -1236,8 +1244,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="16"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
       <c r="B36" s="4" t="s">
         <v>23</v>
       </c>
@@ -1249,8 +1257,8 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="16"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
       <c r="B37" s="4" t="s">
         <v>23</v>
       </c>
@@ -1262,8 +1270,8 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="16"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
       <c r="B38" s="4" t="s">
         <v>23</v>
       </c>
@@ -1275,8 +1283,8 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="16"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
       <c r="B39" s="4" t="s">
         <v>23</v>
       </c>
@@ -1288,93 +1296,93 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="16"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
       <c r="D40"/>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D41"/>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="D42"/>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D43"/>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D44"/>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45"/>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46"/>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47"/>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D48"/>
       <c r="E48"/>
     </row>
-    <row r="49" spans="3:5">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D49"/>
       <c r="E49"/>
     </row>
-    <row r="50" spans="3:5">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D50"/>
       <c r="E50"/>
     </row>
-    <row r="51" spans="3:5">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D51"/>
       <c r="E51"/>
     </row>
-    <row r="52" spans="3:5">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D52"/>
       <c r="E52"/>
     </row>
-    <row r="53" spans="3:5">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D53"/>
       <c r="E53"/>
     </row>
-    <row r="54" spans="3:5">
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D54"/>
       <c r="E54"/>
     </row>
-    <row r="55" spans="3:5">
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D55"/>
       <c r="E55"/>
     </row>
-    <row r="56" spans="3:5">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D56"/>
       <c r="E56"/>
     </row>
-    <row r="57" spans="3:5">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D57"/>
       <c r="E57"/>
     </row>
-    <row r="58" spans="3:5">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D58"/>
       <c r="E58"/>
     </row>
-    <row r="59" spans="3:5">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D59"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="3:5">
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D60"/>
       <c r="E60"/>
     </row>
-    <row r="61" spans="3:5">
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="3"/>
       <c r="E61"/>
     </row>

</xml_diff>